<commit_message>
Work on correcting if species were seeded or not for the subplot data
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11585C87-2231-4F4E-88B8-B5D5858327A7}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41233F1D-4831-4953-852E-F4353478E562}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
     <sheet name="with-site" sheetId="2" r:id="rId2"/>
+    <sheet name="from-Havrilla2020" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
     <author>tc={58C0F180-5C15-4D8D-BA2A-FC6AAC7A1FCC}</author>
   </authors>
   <commentList>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{C94642D0-14F1-47D9-9197-03F961B07019}">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{C94642D0-14F1-47D9-9197-03F961B07019}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -51,7 +52,7 @@
     Was not in original Master.xlsx seed mix list; instead POFE was listed twice. This was added based on the Laushman 2021 RestoreNet guide.</t>
       </text>
     </comment>
-    <comment ref="D33" authorId="1" shapeId="0" xr:uid="{58C0F180-5C15-4D8D-BA2A-FC6AAC7A1FCC}">
+    <comment ref="D32" authorId="1" shapeId="0" xr:uid="{58C0F180-5C15-4D8D-BA2A-FC6AAC7A1FCC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="243">
   <si>
     <t>Family</t>
   </si>
@@ -741,9 +742,6 @@
     <t>Scientific</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Common</t>
   </si>
   <si>
@@ -790,6 +788,12 @@
   </si>
   <si>
     <t>southwestern pricklypoppy</t>
+  </si>
+  <si>
+    <t>CodeOriginal</t>
+  </si>
+  <si>
+    <t>Spiderweb</t>
   </si>
 </sst>
 </file>
@@ -805,12 +809,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -825,8 +841,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,8 +952,8 @@
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -953,7 +971,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10119360" y="464820"/>
-          <a:ext cx="2903220" cy="1668780"/>
+          <a:ext cx="3566160" cy="1668780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,7 +1011,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> don't understand is that PJ is a Utah site, which is ecologically kind of part of the CO Plateau, not near the Chihuahuan Desert.</a:t>
+            <a:t> don't understand is how PJ is a Chihuahuan Desert site, , which is ecologically kind of part of the CO Plateau, not near the Chihuahuan Desert.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1316,10 +1334,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D17" dT="2023-09-06T22:00:52.91" personId="{BFCF90D0-C113-436C-8513-14007208B83F}" id="{C94642D0-14F1-47D9-9197-03F961B07019}">
+  <threadedComment ref="D16" dT="2023-09-06T22:00:52.91" personId="{BFCF90D0-C113-436C-8513-14007208B83F}" id="{C94642D0-14F1-47D9-9197-03F961B07019}">
     <text>Was not in original Master.xlsx seed mix list; instead POFE was listed twice. This was added based on the Laushman 2021 RestoreNet guide.</text>
   </threadedComment>
-  <threadedComment ref="D33" dT="2023-09-06T22:05:15.44" personId="{BFCF90D0-C113-436C-8513-14007208B83F}" id="{58C0F180-5C15-4D8D-BA2A-FC6AAC7A1FCC}">
+  <threadedComment ref="D32" dT="2023-09-06T22:05:15.44" personId="{BFCF90D0-C113-436C-8513-14007208B83F}" id="{58C0F180-5C15-4D8D-BA2A-FC6AAC7A1FCC}">
     <text>Went with "cool" assignment based on Laushman 2021</text>
   </threadedComment>
 </ThreadedComments>
@@ -1331,7 +1349,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD19"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,7 +1364,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1355,24 +1373,24 @@
         <v>224</v>
       </c>
       <c r="D1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" t="s">
         <v>225</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>226</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>227</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>228</v>
-      </c>
-      <c r="H1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1398,7 +1416,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1424,7 +1442,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -1450,7 +1468,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1476,7 +1494,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1502,7 +1520,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1528,7 +1546,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1554,7 +1572,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
@@ -1580,7 +1598,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -1606,7 +1624,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1632,7 +1650,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1658,7 +1676,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1684,7 +1702,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B14" t="s">
         <v>67</v>
@@ -1710,7 +1728,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -1736,7 +1754,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -1762,7 +1780,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -1788,7 +1806,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -1814,7 +1832,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -1840,7 +1858,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -1866,7 +1884,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -1892,7 +1910,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2692,7 +2710,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B53" t="s">
         <v>152</v>
@@ -2718,7 +2736,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -2744,7 +2762,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
@@ -2770,7 +2788,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -2796,7 +2814,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -2819,7 +2837,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -2845,7 +2863,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -2871,7 +2889,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -2897,7 +2915,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
@@ -2923,7 +2941,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B62" t="s">
         <v>49</v>
@@ -2949,7 +2967,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B63" t="s">
         <v>49</v>
@@ -2975,7 +2993,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
@@ -2998,7 +3016,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B65" t="s">
         <v>148</v>
@@ -3024,7 +3042,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B66" t="s">
         <v>152</v>
@@ -3050,7 +3068,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
         <v>139</v>
@@ -3076,7 +3094,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B68" t="s">
         <v>85</v>
@@ -3102,7 +3120,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3128,7 +3146,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
@@ -3154,7 +3172,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
@@ -3180,7 +3198,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
@@ -3206,7 +3224,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -3232,7 +3250,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -3258,7 +3276,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B75" t="s">
         <v>57</v>
@@ -3284,7 +3302,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
@@ -3310,7 +3328,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
@@ -3336,7 +3354,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B78" t="s">
         <v>57</v>
@@ -3362,7 +3380,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
@@ -3388,7 +3406,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B80" t="s">
         <v>112</v>
@@ -3414,7 +3432,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B81" t="s">
         <v>204</v>
@@ -3440,7 +3458,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B82" t="s">
         <v>57</v>
@@ -3466,7 +3484,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B83" t="s">
         <v>85</v>
@@ -3492,7 +3510,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -3518,7 +3536,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
@@ -3544,7 +3562,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B86" t="s">
         <v>124</v>
@@ -3570,7 +3588,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B87" t="s">
         <v>10</v>
@@ -3596,7 +3614,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -3622,7 +3640,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
@@ -3648,7 +3666,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -3674,7 +3692,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
@@ -3700,7 +3718,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
@@ -3723,7 +3741,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
@@ -3749,7 +3767,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
@@ -3775,7 +3793,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B95" t="s">
         <v>112</v>
@@ -3801,7 +3819,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
@@ -3827,7 +3845,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B97" t="s">
         <v>57</v>
@@ -3853,7 +3871,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -3888,11 +3906,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC37BE-5B4E-4F84-9B06-1E5398641E62}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3907,36 +3925,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
         <v>234</v>
-      </c>
-      <c r="B1" t="s">
-        <v>235</v>
       </c>
       <c r="C1" t="s">
         <v>224</v>
       </c>
       <c r="D1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" t="s">
         <v>225</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>226</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>227</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>228</v>
-      </c>
-      <c r="H1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
@@ -3959,10 +3977,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -3985,10 +4003,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -4011,10 +4029,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -4037,10 +4055,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" t="s">
         <v>58</v>
@@ -4063,10 +4081,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
@@ -4089,10 +4107,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -4115,10 +4133,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
@@ -4141,10 +4159,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -4167,10 +4185,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -4193,10 +4211,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C12" t="s">
         <v>64</v>
@@ -4219,10 +4237,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -4234,7 +4252,7 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -4245,534 +4263,531 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14">
-        <v>15.8</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>237</v>
-      </c>
-      <c r="B15" t="s">
-        <v>236</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
+        <v>229</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>19.399999999999999</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>238</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>239</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>240</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>237</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>15.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>230</v>
-      </c>
-      <c r="C17" t="s">
-        <v>239</v>
+        <v>229</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>240</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>238</v>
+        <v>123</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>22.5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
+        <v>229</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
         <v>123</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>22.5</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>230</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
+        <v>229</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H19">
-        <v>21.84</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>230</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
+        <v>229</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>238</v>
+        <v>123</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H20">
-        <v>19.899999999999999</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="G21">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H21">
-        <v>23.15</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H22">
-        <v>18.63</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>230</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
+        <v>229</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>238</v>
+        <v>75</v>
       </c>
       <c r="G23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H23">
-        <v>16.25</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>230</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
+        <v>229</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
         <v>75</v>
       </c>
       <c r="G24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>14.2</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>230</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
+        <v>229</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H25">
-        <v>11.5</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
+        <v>229</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="G26">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H26">
-        <v>19.899999999999999</v>
+        <v>17.72</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>230</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
+        <v>229</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>238</v>
+        <v>123</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H27">
-        <v>17.72</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H28">
-        <v>20.3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
+        <v>229</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>237</v>
       </c>
       <c r="G29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H29">
-        <v>16</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>238</v>
+        <v>75</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H30">
-        <v>17.97</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C31" t="s">
-        <v>54</v>
+        <v>229</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
         <v>75</v>
       </c>
       <c r="G31">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H31">
-        <v>14.2</v>
+        <v>15.95</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>230</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
+        <v>229</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
         <v>75</v>
       </c>
       <c r="G32">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H32">
-        <v>15.95</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>230</v>
-      </c>
-      <c r="C33" t="s">
-        <v>21</v>
+        <v>229</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H33">
-        <v>15.8</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>230</v>
-      </c>
-      <c r="C34" t="s">
-        <v>34</v>
+        <v>229</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
         <v>123</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>20.5</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>230</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
+        <v>229</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="G35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H35">
-        <v>21.6</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="F36" t="s">
-        <v>238</v>
+        <v>94</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36">
-        <v>19.399999999999999</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -4780,22 +4795,22 @@
         <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="E37" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H37">
-        <v>15.5</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -4803,22 +4818,22 @@
         <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>123</v>
       </c>
       <c r="G38">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H38">
-        <v>18.3</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -4826,22 +4841,22 @@
         <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
         <v>123</v>
       </c>
       <c r="G39">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H39">
-        <v>21.1</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -4849,22 +4864,22 @@
         <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>127</v>
+        <v>42</v>
       </c>
       <c r="F40" t="s">
         <v>123</v>
       </c>
       <c r="G40">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H40">
-        <v>19.399999999999999</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -4872,22 +4887,22 @@
         <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F41" t="s">
         <v>123</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H41">
-        <v>21.4</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -4895,22 +4910,22 @@
         <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="F42" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G42">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H42">
-        <v>18.7</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -4918,22 +4933,22 @@
         <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G43">
         <v>3</v>
       </c>
       <c r="H43">
-        <v>17.100000000000001</v>
+        <v>15.9</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -4941,22 +4956,22 @@
         <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="E44" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="F44" t="s">
         <v>94</v>
       </c>
       <c r="G44">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H44">
-        <v>15.9</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -4964,22 +4979,22 @@
         <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="F45" t="s">
         <v>94</v>
       </c>
       <c r="G45">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H45">
-        <v>15.7</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -4987,22 +5002,22 @@
         <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="E46" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="F46" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G46">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H46">
-        <v>15.5</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -5010,22 +5025,22 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E47" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F47" t="s">
         <v>75</v>
       </c>
       <c r="G47">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H47">
-        <v>14.2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -5033,22 +5048,22 @@
         <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F48" t="s">
         <v>75</v>
       </c>
       <c r="G48">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H48">
-        <v>12</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -5056,22 +5071,22 @@
         <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="F49" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G49">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="H49">
-        <v>11.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -5079,22 +5094,19 @@
         <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E50" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F50" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50">
-        <v>13.7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -5102,19 +5114,19 @@
         <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F51" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="G51">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -5122,19 +5134,22 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D52" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="E52" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="F52" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="H52">
+        <v>21.5</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -5142,22 +5157,22 @@
         <v>71</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
       <c r="F53" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G53">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H53">
-        <v>21.5</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -5165,22 +5180,22 @@
         <v>71</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="F54" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G54">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H54">
-        <v>17.399999999999999</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -5188,22 +5203,22 @@
         <v>71</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E55" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F55" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G55">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H55">
-        <v>12.1</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -5211,22 +5226,22 @@
         <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H56">
-        <v>13.3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -5234,22 +5249,22 @@
         <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="F57" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H57">
-        <v>17</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -5257,22 +5272,22 @@
         <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="E58" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="F58" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G58">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H58">
-        <v>14.2</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -5280,22 +5295,22 @@
         <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="F59" t="s">
         <v>104</v>
       </c>
       <c r="G59">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H59">
-        <v>18.100000000000001</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -5303,22 +5318,22 @@
         <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="E60" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="F60" t="s">
         <v>104</v>
       </c>
       <c r="G60">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H60">
-        <v>15.1</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -5326,22 +5341,22 @@
         <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="E61" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="F61" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G61">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H61">
-        <v>16.7</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -5349,22 +5364,22 @@
         <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="F62" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G62">
         <v>14</v>
       </c>
       <c r="H62">
-        <v>11.4</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -5372,22 +5387,22 @@
         <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="E63" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="F63" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G63">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H63">
-        <v>21.7</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -5395,22 +5410,22 @@
         <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="D64" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="E64" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="F64" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="G64">
         <v>4</v>
       </c>
       <c r="H64">
-        <v>12.7</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -5418,88 +5433,88 @@
         <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="F65" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H65">
-        <v>21.6</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="C66" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="D66" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="E66" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="F66" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="G66">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H66">
-        <v>16.899999999999999</v>
+        <v>23.52</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D67" t="s">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="F67" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G67">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H67">
-        <v>23.52</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C68" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D68" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="E68" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="F68" t="s">
         <v>75</v>
       </c>
       <c r="G68">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <v>20.25</v>
@@ -5507,654 +5522,654 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="E69" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="F69" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H69">
-        <v>20.25</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C70" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D70" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E70" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="F70" t="s">
         <v>123</v>
       </c>
       <c r="G70">
-        <v>3</v>
-      </c>
-      <c r="H70">
-        <v>23.38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C71" t="s">
-        <v>179</v>
+        <v>43</v>
       </c>
       <c r="D71" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="E71" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="F71" t="s">
         <v>123</v>
       </c>
       <c r="G71">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="H71">
+        <v>22.5</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C72" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="D72" t="s">
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="E72" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="F72" t="s">
         <v>123</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H72">
-        <v>22.5</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C73" t="s">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="D73" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="E73" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="F73" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G73">
         <v>2</v>
       </c>
       <c r="H73">
-        <v>23.33</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C74" t="s">
-        <v>40</v>
+        <v>173</v>
       </c>
       <c r="D74" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="E74" t="s">
-        <v>42</v>
+        <v>175</v>
       </c>
       <c r="F74" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G74">
         <v>2</v>
       </c>
       <c r="H74">
-        <v>21.84</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C75" t="s">
-        <v>173</v>
+        <v>50</v>
       </c>
       <c r="D75" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
       <c r="E75" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="F75" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G75">
         <v>2</v>
       </c>
       <c r="H75">
-        <v>23.38</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C76" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="D76" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="E76" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="F76" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G76">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H76">
-        <v>19.86</v>
+        <v>23.18</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E77" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F77" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G77">
-        <v>4</v>
-      </c>
-      <c r="H77">
-        <v>23.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D78" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E78" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F78" t="s">
         <v>75</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="H78">
+        <v>21.94</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D79" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E79" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F79" t="s">
         <v>75</v>
       </c>
       <c r="G79">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H79">
-        <v>21.94</v>
+        <v>23.31</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D80" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E80" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="F80" t="s">
         <v>75</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="H80">
-        <v>23.31</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="E81" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F81" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G81">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H81">
-        <v>17.97</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="D82" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="E82" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="F82" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H82">
-        <v>22.96</v>
+        <v>22.89</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C83" t="s">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D83" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
       <c r="E83" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="F83" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G83">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H83">
-        <v>22.89</v>
+        <v>23.46</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C84" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="D84" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="E84" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="F84" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G84">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H84">
-        <v>23.46</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C85" t="s">
-        <v>40</v>
+        <v>218</v>
       </c>
       <c r="D85" t="s">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="E85" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="F85" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G85">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="H85">
-        <v>21.84</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C86" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D86" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E86" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F86" t="s">
         <v>123</v>
       </c>
       <c r="G86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H86">
-        <v>24.88</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C87" t="s">
-        <v>221</v>
+        <v>46</v>
       </c>
       <c r="D87" t="s">
-        <v>222</v>
+        <v>47</v>
       </c>
       <c r="E87" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="F87" t="s">
         <v>123</v>
       </c>
       <c r="G87">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H87">
-        <v>24.2</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C88" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
       <c r="D88" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
       <c r="E88" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F88" t="s">
         <v>123</v>
       </c>
       <c r="G88">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H88">
-        <v>23.15</v>
+        <v>23.97</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C89" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="D89" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="E89" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="F89" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H89">
-        <v>23.97</v>
+        <v>22.87</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C90" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D90" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="E90" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="F90" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H90">
-        <v>22.87</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C91" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="D91" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="E91" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F91" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G91">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H91">
-        <v>23.38</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C92" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D92" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E92" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F92" t="s">
         <v>75</v>
       </c>
       <c r="G92">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H92">
-        <v>21.75</v>
+        <v>20.86</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C93" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="D93" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="E93" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="F93" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H93">
-        <v>20.86</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C94" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D94" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E94" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F94" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G94">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H94">
-        <v>23.5</v>
+        <v>21.66</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C95" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="D95" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="E95" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="F95" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G95">
         <v>2</v>
       </c>
       <c r="H95">
-        <v>21.66</v>
+        <v>23.83</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C96" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="D96" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="E96" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="F96" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G96">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H96">
-        <v>23.83</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C97" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="D97" t="s">
-        <v>162</v>
+        <v>18</v>
       </c>
       <c r="E97" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F97" t="s">
         <v>75</v>
@@ -6163,348 +6178,325 @@
         <v>1.5</v>
       </c>
       <c r="H97">
-        <v>22.96</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="D98" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="E98" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
       <c r="F98" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G98">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="H98">
-        <v>19.399999999999999</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C99" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D99" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E99" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="F99" t="s">
         <v>123</v>
       </c>
       <c r="G99">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H99">
-        <v>21.1</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C100" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="D100" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="E100" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="F100" t="s">
         <v>123</v>
       </c>
       <c r="G100">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H100">
-        <v>19.399999999999999</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C101" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D101" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E101" t="s">
-        <v>42</v>
+        <v>188</v>
       </c>
       <c r="F101" t="s">
         <v>123</v>
       </c>
       <c r="G101">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H101">
-        <v>21.84</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C102" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E102" t="s">
-        <v>188</v>
+        <v>16</v>
       </c>
       <c r="F102" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="G102">
         <v>9</v>
       </c>
       <c r="H102">
-        <v>23.15</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C103" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F103" t="s">
         <v>182</v>
       </c>
       <c r="G103">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H103">
-        <v>18.63</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C104" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D104" t="s">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="E104" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="F104" t="s">
         <v>182</v>
       </c>
       <c r="G104">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H104">
-        <v>16.25</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C105" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="D105" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="E105" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="F105" t="s">
         <v>182</v>
       </c>
       <c r="G105">
-        <v>2</v>
-      </c>
-      <c r="H105">
-        <v>13.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C106" t="s">
-        <v>116</v>
+        <v>185</v>
       </c>
       <c r="D106" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="E106" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
       <c r="F106" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="G106">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="H106">
+        <v>15.97</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C107" t="s">
-        <v>185</v>
+        <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E107" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F107" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="G107">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H107">
-        <v>15.97</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="D108" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="E108" t="s">
-        <v>184</v>
+        <v>115</v>
       </c>
       <c r="F108" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="G108">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H108">
-        <v>17.97</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D109" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E109" t="s">
-        <v>115</v>
+        <v>183</v>
       </c>
       <c r="F109" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="G109">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H109">
-        <v>18.100000000000001</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C110" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="D110" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="E110" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
       <c r="F110" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="G110">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H110">
-        <v>16.7</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C111" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="D111" t="s">
-        <v>135</v>
+        <v>18</v>
       </c>
       <c r="E111" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="F111" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="G111">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H111">
-        <v>21.7</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>232</v>
-      </c>
-      <c r="C112" t="s">
-        <v>17</v>
-      </c>
-      <c r="D112" t="s">
-        <v>18</v>
-      </c>
-      <c r="E112" t="s">
-        <v>19</v>
-      </c>
-      <c r="F112" t="s">
-        <v>182</v>
-      </c>
-      <c r="G112">
-        <v>2</v>
-      </c>
-      <c r="H112">
         <v>19.399999999999999</v>
       </c>
     </row>
@@ -6513,4 +6505,50 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AACCC2-25F8-47C0-AE4C-0CA6CA3F7938}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Look at SpeciesSeeded marked NA separately, because it needs is.na() rather than == NA for filter. Begin with Source col but did not get far
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="535" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30564E69-E7FE-4729-9099-1412083C239E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -4285,9 +4285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AACCC2-25F8-47C0-AE4C-0CA6CA3F7938}">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8109,7 +8109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5849FDA-05E6-480F-8FF0-1C4EF45669E6}">
   <dimension ref="A1:J311"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>

</xml_diff>

<commit_message>
Find aridity index values for RestoreNet sites (took way too long because I didn't realize that loading tidyverse messed up the extract() function and it nearly drove me crazy I died)
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -1024,10 +1024,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4319,8 +4318,8 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5003,10 +5002,10 @@
       <c r="F18" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" t="s">
         <v>303</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" t="s">
         <v>300</v>
       </c>
       <c r="I18" t="s">
@@ -5535,10 +5534,10 @@
       <c r="F32" t="s">
         <v>98</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" t="s">
         <v>303</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" t="s">
         <v>299</v>
       </c>
       <c r="I32" t="s">
@@ -5573,10 +5572,10 @@
       <c r="F33" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" t="s">
         <v>303</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" t="s">
         <v>300</v>
       </c>
       <c r="I33" t="s">
@@ -5611,10 +5610,10 @@
       <c r="F34" t="s">
         <v>101</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" t="s">
         <v>303</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" t="s">
         <v>299</v>
       </c>
       <c r="I34" t="s">
@@ -5649,10 +5648,10 @@
       <c r="F35" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" t="s">
         <v>303</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" t="s">
         <v>300</v>
       </c>
       <c r="I35" t="s">
@@ -5687,10 +5686,10 @@
       <c r="F36" t="s">
         <v>95</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" t="s">
         <v>303</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" t="s">
         <v>299</v>
       </c>
       <c r="I36" t="s">
@@ -5725,10 +5724,10 @@
       <c r="F37" t="s">
         <v>92</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" t="s">
         <v>303</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" t="s">
         <v>299</v>
       </c>
       <c r="I37" t="s">
@@ -5763,10 +5762,10 @@
       <c r="F38" t="s">
         <v>97</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" t="s">
         <v>303</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" t="s">
         <v>300</v>
       </c>
       <c r="I38" t="s">
@@ -5801,10 +5800,10 @@
       <c r="F39" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" t="s">
         <v>303</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" t="s">
         <v>300</v>
       </c>
       <c r="I39" t="s">
@@ -6067,10 +6066,10 @@
       <c r="F46" t="s">
         <v>88</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" t="s">
         <v>303</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" t="s">
         <v>300</v>
       </c>
       <c r="I46" t="s">
@@ -6105,10 +6104,10 @@
       <c r="F47" t="s">
         <v>256</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" t="s">
         <v>303</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" t="s">
         <v>300</v>
       </c>
       <c r="I47" t="s">
@@ -6143,10 +6142,10 @@
       <c r="F48" t="s">
         <v>257</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" t="s">
         <v>303</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" t="s">
         <v>299</v>
       </c>
       <c r="I48" t="s">
@@ -6181,10 +6180,10 @@
       <c r="F49" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" t="s">
         <v>303</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" t="s">
         <v>300</v>
       </c>
       <c r="I49" t="s">
@@ -6216,10 +6215,10 @@
       <c r="F50" t="s">
         <v>258</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" t="s">
         <v>303</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" t="s">
         <v>300</v>
       </c>
       <c r="I50" t="s">
@@ -6254,10 +6253,10 @@
       <c r="F51" t="s">
         <v>74</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" t="s">
         <v>303</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" t="s">
         <v>300</v>
       </c>
       <c r="I51" t="s">
@@ -6292,10 +6291,10 @@
       <c r="F52" t="s">
         <v>259</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" t="s">
         <v>303</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" t="s">
         <v>299</v>
       </c>
       <c r="I52" t="s">
@@ -6596,10 +6595,10 @@
       <c r="F60" t="s">
         <v>88</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" t="s">
         <v>303</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" t="s">
         <v>300</v>
       </c>
       <c r="I60" t="s">
@@ -6634,10 +6633,10 @@
       <c r="F61" t="s">
         <v>256</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" t="s">
         <v>303</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="H61" t="s">
         <v>300</v>
       </c>
       <c r="I61" t="s">
@@ -6672,10 +6671,10 @@
       <c r="F62" t="s">
         <v>257</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" t="s">
         <v>303</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" t="s">
         <v>299</v>
       </c>
       <c r="I62" t="s">
@@ -6710,10 +6709,10 @@
       <c r="F63" t="s">
         <v>91</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" t="s">
         <v>303</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H63" t="s">
         <v>300</v>
       </c>
       <c r="I63" t="s">
@@ -6745,10 +6744,10 @@
       <c r="F64" t="s">
         <v>258</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" t="s">
         <v>303</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H64" t="s">
         <v>300</v>
       </c>
       <c r="I64" t="s">
@@ -6783,10 +6782,10 @@
       <c r="F65" t="s">
         <v>74</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" t="s">
         <v>303</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" t="s">
         <v>300</v>
       </c>
       <c r="I65" t="s">
@@ -6821,10 +6820,10 @@
       <c r="F66" t="s">
         <v>259</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" t="s">
         <v>303</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" t="s">
         <v>299</v>
       </c>
       <c r="I66" t="s">
@@ -7125,10 +7124,10 @@
       <c r="F74" t="s">
         <v>253</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" t="s">
         <v>303</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" t="s">
         <v>300</v>
       </c>
       <c r="I74" t="s">
@@ -7163,10 +7162,10 @@
       <c r="F75" t="s">
         <v>141</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" t="s">
         <v>303</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" t="s">
         <v>300</v>
       </c>
       <c r="I75" t="s">
@@ -7201,10 +7200,10 @@
       <c r="F76" t="s">
         <v>42</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" t="s">
         <v>305</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H76" t="s">
         <v>299</v>
       </c>
       <c r="I76" t="s">
@@ -7239,10 +7238,10 @@
       <c r="F77" t="s">
         <v>274</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G77" t="s">
         <v>303</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H77" t="s">
         <v>299</v>
       </c>
       <c r="I77" t="s">
@@ -7277,10 +7276,10 @@
       <c r="F78" t="s">
         <v>260</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" t="s">
         <v>304</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" t="s">
         <v>299</v>
       </c>
       <c r="I78" t="s">
@@ -7312,10 +7311,10 @@
       <c r="F79" t="s">
         <v>146</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G79" t="s">
         <v>303</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H79" t="s">
         <v>301</v>
       </c>
       <c r="I79" t="s">
@@ -7350,10 +7349,10 @@
       <c r="F80" t="s">
         <v>150</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G80" t="s">
         <v>303</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H80" t="s">
         <v>299</v>
       </c>
       <c r="I80" t="s">
@@ -7388,10 +7387,10 @@
       <c r="F81" t="s">
         <v>137</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" t="s">
         <v>304</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" t="s">
         <v>299</v>
       </c>
       <c r="I81" t="s">
@@ -7426,10 +7425,10 @@
       <c r="F82" t="s">
         <v>173</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G82" t="s">
         <v>304</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H82" t="s">
         <v>299</v>
       </c>
       <c r="I82" t="s">
@@ -7464,10 +7463,10 @@
       <c r="F83" t="s">
         <v>261</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" t="s">
         <v>303</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H83" t="s">
         <v>301</v>
       </c>
       <c r="I83" t="s">
@@ -7502,10 +7501,10 @@
       <c r="F84" t="s">
         <v>176</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" t="s">
         <v>303</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H84" t="s">
         <v>301</v>
       </c>
       <c r="I84" t="s">
@@ -7537,10 +7536,10 @@
       <c r="F85" t="s">
         <v>268</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G85" t="s">
         <v>303</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="H85" t="s">
         <v>301</v>
       </c>
       <c r="I85" t="s">
@@ -7575,10 +7574,10 @@
       <c r="F86" t="s">
         <v>164</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G86" t="s">
         <v>303</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H86" t="s">
         <v>301</v>
       </c>
       <c r="I86" t="s">
@@ -7613,10 +7612,10 @@
       <c r="F87" t="s">
         <v>170</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G87" t="s">
         <v>303</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H87" t="s">
         <v>301</v>
       </c>
       <c r="I87" t="s">
@@ -7651,10 +7650,10 @@
       <c r="F88" t="s">
         <v>161</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" t="s">
         <v>305</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H88" t="s">
         <v>299</v>
       </c>
       <c r="I88" t="s">
@@ -7727,10 +7726,10 @@
       <c r="F90" t="s">
         <v>262</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="G90" t="s">
         <v>303</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="H90" t="s">
         <v>301</v>
       </c>
       <c r="I90" t="s">
@@ -7765,10 +7764,10 @@
       <c r="F91" t="s">
         <v>42</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="G91" t="s">
         <v>305</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="H91" t="s">
         <v>299</v>
       </c>
       <c r="I91" t="s">
@@ -7803,10 +7802,10 @@
       <c r="F92" t="s">
         <v>307</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="G92" t="s">
         <v>303</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="H92" t="s">
         <v>300</v>
       </c>
       <c r="I92" t="s">
@@ -7841,10 +7840,10 @@
       <c r="F93" t="s">
         <v>194</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="G93" t="s">
         <v>304</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="H93" t="s">
         <v>299</v>
       </c>
       <c r="I93" t="s">
@@ -7879,10 +7878,10 @@
       <c r="F94" t="s">
         <v>263</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="G94" t="s">
         <v>303</v>
       </c>
-      <c r="H94" s="2" t="s">
+      <c r="H94" t="s">
         <v>300</v>
       </c>
       <c r="I94" t="s">
@@ -7917,10 +7916,10 @@
       <c r="F95" t="s">
         <v>264</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G95" t="s">
         <v>304</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="H95" t="s">
         <v>299</v>
       </c>
       <c r="I95" t="s">
@@ -7955,10 +7954,10 @@
       <c r="F96" t="s">
         <v>158</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G96" t="s">
         <v>303</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="H96" t="s">
         <v>299</v>
       </c>
       <c r="I96" t="s">
@@ -7993,10 +7992,10 @@
       <c r="F97" t="s">
         <v>19</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="G97" t="s">
         <v>303</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="H97" t="s">
         <v>300</v>
       </c>
       <c r="I97" t="s">
@@ -8031,10 +8030,10 @@
       <c r="F98" t="s">
         <v>255</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G98" t="s">
         <v>303</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="H98" t="s">
         <v>300</v>
       </c>
       <c r="I98" t="s">
@@ -8069,10 +8068,10 @@
       <c r="F99" t="s">
         <v>265</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G99" t="s">
         <v>304</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="H99" t="s">
         <v>300</v>
       </c>
       <c r="I99" t="s">
@@ -8107,10 +8106,10 @@
       <c r="F100" t="s">
         <v>108</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G100" t="s">
         <v>303</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="H100" t="s">
         <v>300</v>
       </c>
       <c r="I100" t="s">
@@ -8145,10 +8144,10 @@
       <c r="F101" t="s">
         <v>182</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G101" t="s">
         <v>303</v>
       </c>
-      <c r="H101" s="2" t="s">
+      <c r="H101" t="s">
         <v>300</v>
       </c>
       <c r="I101" t="s">
@@ -8183,10 +8182,10 @@
       <c r="F102" t="s">
         <v>266</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G102" t="s">
         <v>303</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="H102" t="s">
         <v>301</v>
       </c>
       <c r="I102" t="s">
@@ -8221,10 +8220,10 @@
       <c r="F103" t="s">
         <v>170</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="G103" t="s">
         <v>303</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="H103" t="s">
         <v>301</v>
       </c>
       <c r="I103" t="s">
@@ -8259,10 +8258,10 @@
       <c r="F104" t="s">
         <v>267</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G104" t="s">
         <v>304</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="H104" t="s">
         <v>299</v>
       </c>
       <c r="I104" t="s">
@@ -8335,10 +8334,10 @@
       <c r="F106" t="s">
         <v>16</v>
       </c>
-      <c r="G106" s="2" t="s">
+      <c r="G106" t="s">
         <v>303</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="H106" t="s">
         <v>300</v>
       </c>
       <c r="I106" t="s">
@@ -8373,10 +8372,10 @@
       <c r="F107" t="s">
         <v>4</v>
       </c>
-      <c r="G107" s="2" t="s">
+      <c r="G107" t="s">
         <v>303</v>
       </c>
-      <c r="H107" s="2" t="s">
+      <c r="H107" t="s">
         <v>300</v>
       </c>
       <c r="I107" t="s">
@@ -8411,10 +8410,10 @@
       <c r="F108" t="s">
         <v>95</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="G108" t="s">
         <v>303</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="H108" t="s">
         <v>299</v>
       </c>
       <c r="I108" t="s">
@@ -8449,10 +8448,10 @@
       <c r="F109" t="s">
         <v>115</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="G109" t="s">
         <v>303</v>
       </c>
-      <c r="H109" s="2" t="s">
+      <c r="H109" t="s">
         <v>300</v>
       </c>
       <c r="I109" t="s">
@@ -8484,10 +8483,10 @@
       <c r="F110" t="s">
         <v>178</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="G110" t="s">
         <v>304</v>
       </c>
-      <c r="H110" s="2" t="s">
+      <c r="H110" t="s">
         <v>299</v>
       </c>
       <c r="I110" t="s">
@@ -8522,10 +8521,10 @@
       <c r="F111" t="s">
         <v>177</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="G111" t="s">
         <v>303</v>
       </c>
-      <c r="H111" s="2" t="s">
+      <c r="H111" t="s">
         <v>300</v>
       </c>
       <c r="I111" t="s">
@@ -8560,10 +8559,10 @@
       <c r="F112" t="s">
         <v>19</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="G112" t="s">
         <v>303</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="H112" t="s">
         <v>300</v>
       </c>
       <c r="I112" t="s">
@@ -8598,10 +8597,10 @@
       <c r="F113" t="s">
         <v>255</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="G113" t="s">
         <v>303</v>
       </c>
-      <c r="H113" s="2" t="s">
+      <c r="H113" t="s">
         <v>300</v>
       </c>
       <c r="I113" t="s">
@@ -8636,10 +8635,10 @@
       <c r="F114" t="s">
         <v>181</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="G114" t="s">
         <v>303</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="H114" t="s">
         <v>299</v>
       </c>
       <c r="I114" t="s">
@@ -8674,10 +8673,10 @@
       <c r="F115" t="s">
         <v>42</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="G115" t="s">
         <v>305</v>
       </c>
-      <c r="H115" s="2" t="s">
+      <c r="H115" t="s">
         <v>299</v>
       </c>
       <c r="I115" t="s">
@@ -8712,10 +8711,10 @@
       <c r="F116" t="s">
         <v>182</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G116" t="s">
         <v>303</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="H116" t="s">
         <v>300</v>
       </c>
       <c r="I116" t="s">
@@ -8750,10 +8749,10 @@
       <c r="F117" t="s">
         <v>254</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="G117" t="s">
         <v>303</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="H117" t="s">
         <v>300</v>
       </c>
       <c r="I117" t="s">
@@ -8788,10 +8787,10 @@
       <c r="F118" t="s">
         <v>112</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="G118" t="s">
         <v>303</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="H118" t="s">
         <v>299</v>
       </c>
       <c r="I118" t="s">
@@ -8859,7 +8858,7 @@
   <dimension ref="A1:J311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add code to identify outliers from plots
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="785" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7C645BC-4F53-4654-986E-015704DA9717}"/>
+  <xr:revisionPtr revIDLastSave="787" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4778E7C-176D-43DC-8B09-7228C925AE81}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
@@ -4318,8 +4318,8 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I64" sqref="I64"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
I think I am done with my draft for now and I just want to go to bed. Also add section to identify the most common seeded species to come up with an abbreviated seed mix list
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="787" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4778E7C-176D-43DC-8B09-7228C925AE81}"/>
+  <xr:revisionPtr revIDLastSave="803" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA717705-F87C-49C4-B139-B0770790669C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView minimized="1" xWindow="1080" yWindow="876" windowWidth="13020" windowHeight="11760" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -4317,9 +4317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AACCC2-25F8-47C0-AE4C-0CA6CA3F7938}">
   <dimension ref="A1:L119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
This did not actually change
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4427,8 +4427,8 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J60" sqref="J60:J63"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Identify species doing well in Sonoran Desert mixes
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="877" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57ABF7CF-2365-4AC8-B9E7-14B5416ABD52}"/>
+  <xr:revisionPtr revIDLastSave="896" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B07D61AF-905C-4AE8-8268-ACB3CF351999}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7076" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7076" uniqueCount="313">
   <si>
     <t>Family</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>Projected</t>
+  </si>
+  <si>
+    <t>Rothrock's grama</t>
   </si>
 </sst>
 </file>
@@ -1142,15 +1145,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>81915</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1165,8 +1168,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13064490" y="567690"/>
-          <a:ext cx="3448050" cy="5177790"/>
+          <a:off x="13051155" y="381001"/>
+          <a:ext cx="3451860" cy="5234940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1336,6 +1339,9 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>Code, Duration, and Lifeform according to USDA Plants.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4427,8 +4433,8 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8213,7 +8219,7 @@
         <v>216</v>
       </c>
       <c r="F100" t="s">
-        <v>108</v>
+        <v>312</v>
       </c>
       <c r="G100" t="s">
         <v>303</v>

</xml_diff>

<commit_message>
Continue identifying outliers in Sonoran and graph Seeded only by PlotMix_Climate and Duration
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="896" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B07D61AF-905C-4AE8-8268-ACB3CF351999}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView minimized="1" xWindow="3036" yWindow="420" windowWidth="17256" windowHeight="8868" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -4433,8 +4433,8 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix N AZ species of interest; continue investigating species of interest at both N AZ and Sonoran Desert
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="920" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77445C1B-65DA-4390-A55D-C33432C71040}"/>
+  <xr:revisionPtr revIDLastSave="922" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84B82025-A6A7-4364-AA6D-DEEC8159A41C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -1040,11 +1040,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4435,8 +4433,8 @@
   <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7446,7 +7444,7 @@
       <c r="A74" t="s">
         <v>224</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" t="s">
         <v>224</v>
       </c>
       <c r="C74" t="s">
@@ -7487,7 +7485,7 @@
       <c r="A75" t="s">
         <v>224</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" t="s">
         <v>224</v>
       </c>
       <c r="C75" t="s">
@@ -7528,7 +7526,7 @@
       <c r="A76" t="s">
         <v>224</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" t="s">
         <v>224</v>
       </c>
       <c r="C76" t="s">
@@ -7569,7 +7567,7 @@
       <c r="A77" t="s">
         <v>224</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" t="s">
         <v>224</v>
       </c>
       <c r="C77" t="s">
@@ -7610,7 +7608,7 @@
       <c r="A78" t="s">
         <v>224</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" t="s">
         <v>224</v>
       </c>
       <c r="C78" t="s">
@@ -7648,7 +7646,7 @@
       <c r="A79" t="s">
         <v>224</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" t="s">
         <v>224</v>
       </c>
       <c r="C79" t="s">
@@ -7689,7 +7687,7 @@
       <c r="A80" t="s">
         <v>224</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" t="s">
         <v>224</v>
       </c>
       <c r="C80" t="s">
@@ -7730,7 +7728,7 @@
       <c r="A81" t="s">
         <v>224</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" t="s">
         <v>224</v>
       </c>
       <c r="C81" t="s">
@@ -7771,7 +7769,7 @@
       <c r="A82" t="s">
         <v>224</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" t="s">
         <v>224</v>
       </c>
       <c r="C82" t="s">
@@ -7812,7 +7810,7 @@
       <c r="A83" t="s">
         <v>224</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" t="s">
         <v>224</v>
       </c>
       <c r="C83" t="s">
@@ -7853,7 +7851,7 @@
       <c r="A84" t="s">
         <v>224</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" t="s">
         <v>224</v>
       </c>
       <c r="C84" t="s">
@@ -7891,7 +7889,7 @@
       <c r="A85" t="s">
         <v>224</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" t="s">
         <v>224</v>
       </c>
       <c r="C85" t="s">
@@ -7932,7 +7930,7 @@
       <c r="A86" t="s">
         <v>224</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" t="s">
         <v>224</v>
       </c>
       <c r="C86" t="s">
@@ -7973,7 +7971,7 @@
       <c r="A87" t="s">
         <v>224</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" t="s">
         <v>224</v>
       </c>
       <c r="C87" t="s">
@@ -8014,7 +8012,7 @@
       <c r="A88" t="s">
         <v>224</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" t="s">
         <v>224</v>
       </c>
       <c r="C88" t="s">
@@ -8055,7 +8053,7 @@
       <c r="A89" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="1" t="s">
         <v>224</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -8096,7 +8094,7 @@
       <c r="A90" t="s">
         <v>226</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" t="s">
         <v>226</v>
       </c>
       <c r="C90" t="s">
@@ -8137,7 +8135,7 @@
       <c r="A91" t="s">
         <v>226</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" t="s">
         <v>226</v>
       </c>
       <c r="C91" t="s">
@@ -8178,7 +8176,7 @@
       <c r="A92" t="s">
         <v>226</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" t="s">
         <v>226</v>
       </c>
       <c r="C92" t="s">
@@ -8219,7 +8217,7 @@
       <c r="A93" t="s">
         <v>226</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" t="s">
         <v>226</v>
       </c>
       <c r="C93" t="s">
@@ -8260,7 +8258,7 @@
       <c r="A94" t="s">
         <v>226</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" t="s">
         <v>226</v>
       </c>
       <c r="C94" t="s">
@@ -8301,7 +8299,7 @@
       <c r="A95" t="s">
         <v>226</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" t="s">
         <v>226</v>
       </c>
       <c r="C95" t="s">
@@ -8342,7 +8340,7 @@
       <c r="A96" t="s">
         <v>226</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" t="s">
         <v>226</v>
       </c>
       <c r="C96" t="s">
@@ -8383,7 +8381,7 @@
       <c r="A97" t="s">
         <v>226</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" t="s">
         <v>226</v>
       </c>
       <c r="C97" t="s">
@@ -8424,7 +8422,7 @@
       <c r="A98" t="s">
         <v>226</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" t="s">
         <v>226</v>
       </c>
       <c r="C98" t="s">
@@ -8465,7 +8463,7 @@
       <c r="A99" t="s">
         <v>226</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" t="s">
         <v>226</v>
       </c>
       <c r="C99" t="s">
@@ -8506,7 +8504,7 @@
       <c r="A100" t="s">
         <v>226</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" t="s">
         <v>226</v>
       </c>
       <c r="C100" t="s">
@@ -8547,7 +8545,7 @@
       <c r="A101" t="s">
         <v>226</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" t="s">
         <v>226</v>
       </c>
       <c r="C101" t="s">
@@ -8588,7 +8586,7 @@
       <c r="A102" t="s">
         <v>226</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" t="s">
         <v>226</v>
       </c>
       <c r="C102" t="s">
@@ -8629,7 +8627,7 @@
       <c r="A103" t="s">
         <v>226</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" t="s">
         <v>226</v>
       </c>
       <c r="C103" t="s">
@@ -8670,7 +8668,7 @@
       <c r="A104" t="s">
         <v>226</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" t="s">
         <v>226</v>
       </c>
       <c r="C104" t="s">
@@ -8711,7 +8709,7 @@
       <c r="A105" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="1" t="s">
         <v>226</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -8752,7 +8750,7 @@
       <c r="A106" t="s">
         <v>225</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" t="s">
         <v>225</v>
       </c>
       <c r="C106" t="s">
@@ -8793,7 +8791,7 @@
       <c r="A107" t="s">
         <v>225</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" t="s">
         <v>225</v>
       </c>
       <c r="C107" t="s">
@@ -8834,7 +8832,7 @@
       <c r="A108" t="s">
         <v>225</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" t="s">
         <v>225</v>
       </c>
       <c r="C108" t="s">
@@ -8875,7 +8873,7 @@
       <c r="A109" t="s">
         <v>225</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" t="s">
         <v>225</v>
       </c>
       <c r="C109" t="s">
@@ -8913,7 +8911,7 @@
       <c r="A110" t="s">
         <v>225</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" t="s">
         <v>225</v>
       </c>
       <c r="C110" t="s">
@@ -8954,7 +8952,7 @@
       <c r="A111" t="s">
         <v>225</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" t="s">
         <v>225</v>
       </c>
       <c r="C111" t="s">
@@ -8995,7 +8993,7 @@
       <c r="A112" t="s">
         <v>225</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" t="s">
         <v>225</v>
       </c>
       <c r="C112" t="s">
@@ -9036,7 +9034,7 @@
       <c r="A113" t="s">
         <v>225</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" t="s">
         <v>225</v>
       </c>
       <c r="C113" t="s">
@@ -9077,7 +9075,7 @@
       <c r="A114" t="s">
         <v>225</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" t="s">
         <v>225</v>
       </c>
       <c r="C114" t="s">
@@ -9118,7 +9116,7 @@
       <c r="A115" t="s">
         <v>225</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" t="s">
         <v>225</v>
       </c>
       <c r="C115" t="s">
@@ -9159,7 +9157,7 @@
       <c r="A116" t="s">
         <v>225</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" t="s">
         <v>225</v>
       </c>
       <c r="C116" t="s">
@@ -9200,7 +9198,7 @@
       <c r="A117" t="s">
         <v>225</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" t="s">
         <v>225</v>
       </c>
       <c r="C117" t="s">
@@ -9241,7 +9239,7 @@
       <c r="A118" t="s">
         <v>225</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" t="s">
         <v>225</v>
       </c>
       <c r="C118" t="s">
@@ -9282,7 +9280,7 @@
       <c r="A119" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C119" s="1" t="s">

</xml_diff>

<commit_message>
Realized I had done seeded version 1 & 2 wrong for Sonoran Desert, and now the frequency rates make a lot more sense
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="922" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84B82025-A6A7-4364-AA6D-DEEC8159A41C}"/>
+  <xr:revisionPtr revIDLastSave="929" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56521DEA-C85B-4FC6-AC42-704F22EE6396}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
@@ -1002,10 +1002,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1040,9 +1046,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4433,8 +4441,8 @@
   <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5453,7 +5461,7 @@
       <c r="E25" t="s">
         <v>117</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>118</v>
       </c>
       <c r="G25" t="s">
@@ -5494,7 +5502,7 @@
       <c r="E26" t="s">
         <v>124</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>125</v>
       </c>
       <c r="G26" t="s">
@@ -5535,7 +5543,7 @@
       <c r="E27" t="s">
         <v>121</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>122</v>
       </c>
       <c r="G27" t="s">
@@ -5576,7 +5584,7 @@
       <c r="E28" t="s">
         <v>40</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G28" t="s">
@@ -5617,7 +5625,7 @@
       <c r="E29" t="s">
         <v>46</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G29" t="s">
@@ -5658,7 +5666,7 @@
       <c r="E30" t="s">
         <v>127</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>128</v>
       </c>
       <c r="G30" t="s">
@@ -5699,7 +5707,7 @@
       <c r="E31" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="3" t="s">
         <v>131</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -5740,7 +5748,7 @@
       <c r="E32" t="s">
         <v>61</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G32" t="s">
@@ -5781,7 +5789,7 @@
       <c r="E33" t="s">
         <v>14</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G33" t="s">
@@ -5822,7 +5830,7 @@
       <c r="E34" t="s">
         <v>99</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G34" t="s">
@@ -5863,7 +5871,7 @@
       <c r="E35" t="s">
         <v>2</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G35" t="s">
@@ -5904,7 +5912,7 @@
       <c r="E36" t="s">
         <v>93</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G36" t="s">
@@ -5945,7 +5953,7 @@
       <c r="E37" t="s">
         <v>68</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G37" t="s">
@@ -5986,7 +5994,7 @@
       <c r="E38" t="s">
         <v>96</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G38" t="s">
@@ -6027,7 +6035,7 @@
       <c r="E39" t="s">
         <v>106</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G39" t="s">
@@ -6068,7 +6076,7 @@
       <c r="E40" t="s">
         <v>7</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G40" t="s">
@@ -6109,7 +6117,7 @@
       <c r="E41" t="s">
         <v>11</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G41" t="s">
@@ -6150,7 +6158,7 @@
       <c r="E42" t="s">
         <v>110</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G42" t="s">
@@ -6191,7 +6199,7 @@
       <c r="E43" t="s">
         <v>64</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G43" t="s">
@@ -6232,7 +6240,7 @@
       <c r="E44" t="s">
         <v>102</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G44" t="s">
@@ -6273,7 +6281,7 @@
       <c r="E45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -6314,7 +6322,7 @@
       <c r="E46" t="s">
         <v>58</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G46" t="s">
@@ -6355,7 +6363,7 @@
       <c r="E47" t="s">
         <v>78</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G47" t="s">
@@ -6396,7 +6404,7 @@
       <c r="E48" t="s">
         <v>75</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G48" t="s">
@@ -6437,7 +6445,7 @@
       <c r="E49" t="s">
         <v>89</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G49" t="s">
@@ -6475,7 +6483,7 @@
       <c r="E50" t="s">
         <v>81</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G50" t="s">
@@ -6516,7 +6524,7 @@
       <c r="E51" t="s">
         <v>72</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G51" t="s">

</xml_diff>

<commit_message>
Identify low performing seeded species
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="929" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56521DEA-C85B-4FC6-AC42-704F22EE6396}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -4441,8 +4441,8 @@
   <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Remove outliers from N AZ weedy fig
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1014" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B4B36E-E7DB-433B-883F-219CE80B2DC6}"/>
+  <xr:revisionPtr revIDLastSave="1062" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AB3E0C2-F44D-4375-9BBE-AEFBEDD0FBDD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7864" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7951" uniqueCount="336">
   <si>
     <t>Family</t>
   </si>
@@ -1053,16 +1053,19 @@
     <t>Seeding rate (lbs/acre)</t>
   </si>
   <si>
-    <t>Current_BR</t>
-  </si>
-  <si>
-    <t>Projected_BR</t>
-  </si>
-  <si>
-    <t>Current_MA</t>
-  </si>
-  <si>
-    <t>Projected_MA</t>
+    <t>Climate adaptation</t>
+  </si>
+  <si>
+    <t>Cool_BR</t>
+  </si>
+  <si>
+    <t>Warm_BR</t>
+  </si>
+  <si>
+    <t>Med_MA</t>
+  </si>
+  <si>
+    <t>Warm_MA</t>
   </si>
 </sst>
 </file>
@@ -1113,19 +1116,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1939,8 +1939,8 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4516,8 +4516,8 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28053,68 +28053,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3956EC7-86B1-4603-B84C-C9BA64C80C6D}">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:K87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="4" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>313</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>316</v>
       </c>
       <c r="C2" t="s">
@@ -28138,18 +28142,21 @@
       <c r="I2" t="s">
         <v>317</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K2">
         <v>3</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>313</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>316</v>
       </c>
       <c r="C3" t="s">
@@ -28173,18 +28180,21 @@
       <c r="I3" t="s">
         <v>317</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>313</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>316</v>
       </c>
       <c r="C4" t="s">
@@ -28208,18 +28218,21 @@
       <c r="I4" t="s">
         <v>317</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="s">
+        <v>310</v>
+      </c>
+      <c r="K4">
         <v>5</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>313</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>316</v>
       </c>
       <c r="C5" t="s">
@@ -28243,18 +28256,21 @@
       <c r="I5" t="s">
         <v>317</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K5">
         <v>3</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>316</v>
       </c>
       <c r="C6" t="s">
@@ -28278,18 +28294,21 @@
       <c r="I6" t="s">
         <v>317</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="s">
+        <v>310</v>
+      </c>
+      <c r="K6">
         <v>12</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>15.1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>313</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>316</v>
       </c>
       <c r="C7" t="s">
@@ -28313,18 +28332,21 @@
       <c r="I7" t="s">
         <v>317</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="s">
+        <v>310</v>
+      </c>
+      <c r="K7">
         <v>4</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>16.7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>313</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>316</v>
       </c>
       <c r="C8" t="s">
@@ -28348,18 +28370,21 @@
       <c r="I8" t="s">
         <v>317</v>
       </c>
-      <c r="J8">
+      <c r="J8" t="s">
+        <v>310</v>
+      </c>
+      <c r="K8">
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>313</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>316</v>
       </c>
       <c r="C9" t="s">
@@ -28383,18 +28408,21 @@
       <c r="I9" t="s">
         <v>318</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="s">
+        <v>311</v>
+      </c>
+      <c r="K9">
         <v>12</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>18.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>313</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>316</v>
       </c>
       <c r="C10" t="s">
@@ -28418,18 +28446,21 @@
       <c r="I10" t="s">
         <v>318</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="s">
+        <v>311</v>
+      </c>
+      <c r="K10">
         <v>6</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>21.1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>313</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>316</v>
       </c>
       <c r="C11" t="s">
@@ -28453,18 +28484,21 @@
       <c r="I11" t="s">
         <v>318</v>
       </c>
-      <c r="J11">
+      <c r="J11" t="s">
+        <v>311</v>
+      </c>
+      <c r="K11">
         <v>12</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>313</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>316</v>
       </c>
       <c r="C12" t="s">
@@ -28488,18 +28522,21 @@
       <c r="I12" t="s">
         <v>318</v>
       </c>
-      <c r="J12">
+      <c r="J12" t="s">
+        <v>311</v>
+      </c>
+      <c r="K12">
         <v>2</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>21.4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>313</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>316</v>
       </c>
       <c r="C13" t="s">
@@ -28523,18 +28560,21 @@
       <c r="I13" t="s">
         <v>318</v>
       </c>
-      <c r="J13">
+      <c r="J13" t="s">
+        <v>311</v>
+      </c>
+      <c r="K13">
         <v>9</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>18.7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>313</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>316</v>
       </c>
       <c r="C14" t="s">
@@ -28558,18 +28598,21 @@
       <c r="I14" t="s">
         <v>318</v>
       </c>
-      <c r="J14">
+      <c r="J14" t="s">
+        <v>311</v>
+      </c>
+      <c r="K14">
         <v>9</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>21.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>316</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -28593,18 +28636,21 @@
       <c r="I15" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="K15" s="1">
         <v>14</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>21.7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>313</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>316</v>
       </c>
       <c r="C16" t="s">
@@ -28628,18 +28674,21 @@
       <c r="I16" t="s">
         <v>319</v>
       </c>
-      <c r="J16">
-        <v>1</v>
+      <c r="J16" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
         <v>15.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>313</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>316</v>
       </c>
       <c r="C17" t="s">
@@ -28663,18 +28712,21 @@
       <c r="I17" t="s">
         <v>319</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K17">
         <v>3</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>15.9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>313</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>316</v>
       </c>
       <c r="C18" t="s">
@@ -28698,18 +28750,21 @@
       <c r="I18" t="s">
         <v>319</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K18">
         <v>12</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>15.7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>316</v>
       </c>
       <c r="C19" t="s">
@@ -28733,18 +28788,21 @@
       <c r="I19" t="s">
         <v>319</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K19">
         <v>6</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>15.5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>313</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>316</v>
       </c>
       <c r="C20" t="s">
@@ -28768,18 +28826,21 @@
       <c r="I20" t="s">
         <v>319</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K20">
         <v>2</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>13.7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>313</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>316</v>
       </c>
       <c r="C21" t="s">
@@ -28803,18 +28864,21 @@
       <c r="I21" t="s">
         <v>319</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K21">
         <v>6</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>13.3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>313</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>316</v>
       </c>
       <c r="C22" t="s">
@@ -28838,18 +28902,21 @@
       <c r="I22" t="s">
         <v>319</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K22">
         <v>16</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>14.2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>313</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>316</v>
       </c>
       <c r="C23" t="s">
@@ -28873,18 +28940,21 @@
       <c r="I23" t="s">
         <v>317</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K23">
         <v>3</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>313</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>316</v>
       </c>
       <c r="C24" t="s">
@@ -28908,18 +28978,21 @@
       <c r="I24" t="s">
         <v>317</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K24">
         <v>6</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>313</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>316</v>
       </c>
       <c r="C25" t="s">
@@ -28943,18 +29016,21 @@
       <c r="I25" t="s">
         <v>317</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K25">
         <v>5</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>313</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>316</v>
       </c>
       <c r="C26" t="s">
@@ -28978,18 +29054,21 @@
       <c r="I26" t="s">
         <v>317</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K26">
         <v>3</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>313</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>316</v>
       </c>
       <c r="C27" t="s">
@@ -29013,18 +29092,21 @@
       <c r="I27" t="s">
         <v>317</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K27">
         <v>12</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>15.1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>313</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s">
         <v>316</v>
       </c>
       <c r="C28" t="s">
@@ -29048,18 +29130,21 @@
       <c r="I28" t="s">
         <v>317</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K28">
         <v>4</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>16.7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="1" t="s">
         <v>316</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -29083,14 +29168,17 @@
       <c r="I29" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="K29" s="1">
         <v>2</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>313</v>
       </c>
@@ -29118,14 +29206,17 @@
       <c r="I30" t="s">
         <v>320</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K30">
         <v>10</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>14.2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>313</v>
       </c>
@@ -29153,14 +29244,17 @@
       <c r="I31" t="s">
         <v>320</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K31">
         <v>15</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>313</v>
       </c>
@@ -29188,14 +29282,17 @@
       <c r="I32" t="s">
         <v>320</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K32">
         <v>25</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>11.7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>313</v>
       </c>
@@ -29223,14 +29320,17 @@
       <c r="I33" t="s">
         <v>320</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K33">
         <v>14</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>313</v>
       </c>
@@ -29258,14 +29358,17 @@
       <c r="I34" t="s">
         <v>320</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K34">
         <v>11</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>12.1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>313</v>
       </c>
@@ -29293,14 +29396,17 @@
       <c r="I35" t="s">
         <v>320</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K35">
         <v>14</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>11.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>313</v>
       </c>
@@ -29328,14 +29434,17 @@
       <c r="I36" t="s">
         <v>320</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K36">
         <v>4</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>12.7</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>313</v>
       </c>
@@ -29363,14 +29472,17 @@
       <c r="I37" t="s">
         <v>319</v>
       </c>
-      <c r="J37">
-        <v>1</v>
+      <c r="J37" s="5" t="s">
+        <v>311</v>
       </c>
       <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
         <v>15.5</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>313</v>
       </c>
@@ -29398,14 +29510,17 @@
       <c r="I38" t="s">
         <v>319</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K38">
         <v>3</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>15.9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>313</v>
       </c>
@@ -29433,14 +29548,17 @@
       <c r="I39" t="s">
         <v>319</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K39">
         <v>12</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>15.7</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>313</v>
       </c>
@@ -29468,14 +29586,17 @@
       <c r="I40" t="s">
         <v>319</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K40">
         <v>6</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>15.5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>313</v>
       </c>
@@ -29503,14 +29624,17 @@
       <c r="I41" t="s">
         <v>319</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K41">
         <v>2</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>13.7</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>313</v>
       </c>
@@ -29538,14 +29662,17 @@
       <c r="I42" t="s">
         <v>319</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K42">
         <v>6</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>13.3</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>313</v>
       </c>
@@ -29573,14 +29700,17 @@
       <c r="I43" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="K43" s="1">
         <v>16</v>
       </c>
-      <c r="K43" s="1">
+      <c r="L43" s="1">
         <v>14.2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>313</v>
       </c>
@@ -29608,14 +29738,17 @@
       <c r="I44" t="s">
         <v>320</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K44">
         <v>10</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>14.2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>313</v>
       </c>
@@ -29643,14 +29776,17 @@
       <c r="I45" t="s">
         <v>320</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K45">
         <v>15</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>313</v>
       </c>
@@ -29678,14 +29814,17 @@
       <c r="I46" t="s">
         <v>320</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K46">
         <v>25</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>11.7</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>313</v>
       </c>
@@ -29713,14 +29852,17 @@
       <c r="I47" t="s">
         <v>320</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K47">
         <v>14</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>313</v>
       </c>
@@ -29748,14 +29890,17 @@
       <c r="I48" t="s">
         <v>320</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K48">
         <v>11</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>12.1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>313</v>
       </c>
@@ -29783,14 +29928,17 @@
       <c r="I49" t="s">
         <v>320</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K49">
         <v>14</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>11.4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>313</v>
       </c>
@@ -29818,14 +29966,17 @@
       <c r="I50" t="s">
         <v>320</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K50">
         <v>4</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>12.7</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>313</v>
       </c>
@@ -29853,14 +30004,17 @@
       <c r="I51" t="s">
         <v>318</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K51">
         <v>12</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>18.3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>313</v>
       </c>
@@ -29888,14 +30042,17 @@
       <c r="I52" t="s">
         <v>318</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K52">
         <v>6</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>21.1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>313</v>
       </c>
@@ -29923,14 +30080,17 @@
       <c r="I53" t="s">
         <v>318</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K53">
         <v>12</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>313</v>
       </c>
@@ -29958,14 +30118,17 @@
       <c r="I54" t="s">
         <v>318</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K54">
         <v>2</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>21.4</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>313</v>
       </c>
@@ -29993,14 +30156,17 @@
       <c r="I55" t="s">
         <v>318</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K55">
         <v>9</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>18.7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>313</v>
       </c>
@@ -30028,15 +30194,18 @@
       <c r="I56" t="s">
         <v>318</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="K56">
         <v>9</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>21.5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>313</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -30063,15 +30232,18 @@
       <c r="I57" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="J57" s="1">
+      <c r="J57" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="K57" s="1">
         <v>14</v>
       </c>
-      <c r="K57" s="1">
+      <c r="L57" s="1">
         <v>21.7</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>325</v>
       </c>
       <c r="B58" t="s">
@@ -30096,17 +30268,20 @@
         <v>301</v>
       </c>
       <c r="I58" t="s">
-        <v>331</v>
-      </c>
-      <c r="J58">
+        <v>332</v>
+      </c>
+      <c r="J58" t="s">
+        <v>310</v>
+      </c>
+      <c r="K58">
         <v>5</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>22.89</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>325</v>
       </c>
       <c r="B59" t="s">
@@ -30131,17 +30306,20 @@
         <v>299</v>
       </c>
       <c r="I59" t="s">
-        <v>331</v>
-      </c>
-      <c r="J59">
+        <v>332</v>
+      </c>
+      <c r="J59" t="s">
+        <v>310</v>
+      </c>
+      <c r="K59">
         <v>1.5</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>21.84</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>325</v>
       </c>
       <c r="B60" t="s">
@@ -30166,17 +30344,20 @@
         <v>300</v>
       </c>
       <c r="I60" t="s">
-        <v>331</v>
-      </c>
-      <c r="J60">
+        <v>332</v>
+      </c>
+      <c r="J60" t="s">
+        <v>310</v>
+      </c>
+      <c r="K60">
         <v>4</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>22.87</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>325</v>
       </c>
       <c r="B61" t="s">
@@ -30201,17 +30382,20 @@
         <v>299</v>
       </c>
       <c r="I61" t="s">
-        <v>331</v>
-      </c>
-      <c r="J61">
+        <v>332</v>
+      </c>
+      <c r="J61" t="s">
+        <v>310</v>
+      </c>
+      <c r="K61">
         <v>3</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>21.75</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>325</v>
       </c>
       <c r="B62" t="s">
@@ -30236,17 +30420,20 @@
         <v>300</v>
       </c>
       <c r="I62" t="s">
-        <v>331</v>
-      </c>
-      <c r="J62">
-        <v>1</v>
+        <v>332</v>
+      </c>
+      <c r="J62" t="s">
+        <v>310</v>
       </c>
       <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
         <v>20.86</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>325</v>
       </c>
       <c r="B63" t="s">
@@ -30271,17 +30458,20 @@
         <v>299</v>
       </c>
       <c r="I63" t="s">
-        <v>331</v>
-      </c>
-      <c r="J63">
+        <v>332</v>
+      </c>
+      <c r="J63" t="s">
+        <v>310</v>
+      </c>
+      <c r="K63">
         <v>2</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>21.66</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>325</v>
       </c>
       <c r="B64" t="s">
@@ -30306,17 +30496,20 @@
         <v>299</v>
       </c>
       <c r="I64" t="s">
-        <v>331</v>
-      </c>
-      <c r="J64">
+        <v>332</v>
+      </c>
+      <c r="J64" t="s">
+        <v>310</v>
+      </c>
+      <c r="K64">
         <v>1.5</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <v>22.96</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>325</v>
       </c>
       <c r="B65" t="s">
@@ -30341,17 +30534,20 @@
         <v>300</v>
       </c>
       <c r="I65" t="s">
-        <v>331</v>
-      </c>
-      <c r="J65">
+        <v>332</v>
+      </c>
+      <c r="J65" t="s">
+        <v>310</v>
+      </c>
+      <c r="K65">
         <v>1.5</v>
       </c>
-      <c r="K65">
+      <c r="L65">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>325</v>
       </c>
       <c r="B66" t="s">
@@ -30376,17 +30572,20 @@
         <v>300</v>
       </c>
       <c r="I66" t="s">
-        <v>332</v>
-      </c>
-      <c r="J66">
+        <v>333</v>
+      </c>
+      <c r="J66" t="s">
+        <v>311</v>
+      </c>
+      <c r="K66">
         <v>3</v>
       </c>
-      <c r="K66">
+      <c r="L66">
         <v>23.46</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>325</v>
       </c>
       <c r="B67" t="s">
@@ -30411,17 +30610,20 @@
         <v>300</v>
       </c>
       <c r="I67" t="s">
-        <v>332</v>
-      </c>
-      <c r="J67">
+        <v>333</v>
+      </c>
+      <c r="J67" t="s">
+        <v>311</v>
+      </c>
+      <c r="K67">
         <v>3</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <v>24.88</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>325</v>
       </c>
       <c r="B68" t="s">
@@ -30446,17 +30648,20 @@
         <v>300</v>
       </c>
       <c r="I68" t="s">
-        <v>332</v>
-      </c>
-      <c r="J68">
+        <v>333</v>
+      </c>
+      <c r="J68" t="s">
+        <v>311</v>
+      </c>
+      <c r="K68">
         <v>2</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <v>24.2</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="7" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>325</v>
       </c>
       <c r="B69" t="s">
@@ -30481,17 +30686,20 @@
         <v>300</v>
       </c>
       <c r="I69" t="s">
-        <v>332</v>
-      </c>
-      <c r="J69">
+        <v>333</v>
+      </c>
+      <c r="J69" t="s">
+        <v>311</v>
+      </c>
+      <c r="K69">
         <v>3</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>23.15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>325</v>
       </c>
       <c r="B70" t="s">
@@ -30516,17 +30724,20 @@
         <v>301</v>
       </c>
       <c r="I70" t="s">
-        <v>332</v>
-      </c>
-      <c r="J70">
+        <v>333</v>
+      </c>
+      <c r="J70" t="s">
+        <v>311</v>
+      </c>
+      <c r="K70">
         <v>5</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>23.97</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="7" t="s">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>325</v>
       </c>
       <c r="B71" t="s">
@@ -30551,17 +30762,20 @@
         <v>301</v>
       </c>
       <c r="I71" t="s">
-        <v>332</v>
-      </c>
-      <c r="J71">
+        <v>333</v>
+      </c>
+      <c r="J71" t="s">
+        <v>311</v>
+      </c>
+      <c r="K71">
         <v>2</v>
       </c>
-      <c r="K71">
+      <c r="L71">
         <v>23.38</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="7" t="s">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>325</v>
       </c>
       <c r="B72" t="s">
@@ -30586,17 +30800,20 @@
         <v>299</v>
       </c>
       <c r="I72" t="s">
-        <v>332</v>
-      </c>
-      <c r="J72">
+        <v>333</v>
+      </c>
+      <c r="J72" t="s">
+        <v>311</v>
+      </c>
+      <c r="K72">
         <v>1.5</v>
       </c>
-      <c r="K72">
+      <c r="L72">
         <v>23.5</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A73" s="8" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>325</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -30621,17 +30838,20 @@
         <v>299</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="J73" s="1">
+        <v>333</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="K73" s="1">
         <v>2</v>
       </c>
-      <c r="K73" s="1">
+      <c r="L73" s="1">
         <v>23.83</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>325</v>
       </c>
       <c r="B74" t="s">
@@ -30656,17 +30876,20 @@
         <v>300</v>
       </c>
       <c r="I74" t="s">
-        <v>333</v>
-      </c>
-      <c r="J74">
+        <v>334</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K74">
         <v>9</v>
       </c>
-      <c r="K74">
+      <c r="L74">
         <v>18.63</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A75" s="7" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>325</v>
       </c>
       <c r="B75" t="s">
@@ -30691,17 +30914,20 @@
         <v>300</v>
       </c>
       <c r="I75" t="s">
-        <v>333</v>
-      </c>
-      <c r="J75">
+        <v>334</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K75">
         <v>12</v>
       </c>
-      <c r="K75">
+      <c r="L75">
         <v>16.25</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>325</v>
       </c>
       <c r="B76" t="s">
@@ -30726,17 +30952,20 @@
         <v>299</v>
       </c>
       <c r="I76" t="s">
-        <v>333</v>
-      </c>
-      <c r="J76">
+        <v>334</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K76">
         <v>2</v>
       </c>
-      <c r="K76">
+      <c r="L76">
         <v>13.7</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>325</v>
       </c>
       <c r="B77" t="s">
@@ -30761,17 +30990,20 @@
         <v>300</v>
       </c>
       <c r="I77" t="s">
-        <v>333</v>
-      </c>
-      <c r="J77">
+        <v>334</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K77">
         <v>3</v>
       </c>
-      <c r="K77" t="s">
+      <c r="L77" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>325</v>
       </c>
       <c r="B78" t="s">
@@ -30796,17 +31028,20 @@
         <v>299</v>
       </c>
       <c r="I78" t="s">
-        <v>333</v>
-      </c>
-      <c r="J78">
+        <v>334</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K78">
         <v>5</v>
       </c>
-      <c r="K78">
+      <c r="L78">
         <v>17.97</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A79" s="7" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>325</v>
       </c>
       <c r="B79" t="s">
@@ -30831,17 +31066,20 @@
         <v>300</v>
       </c>
       <c r="I79" t="s">
-        <v>333</v>
-      </c>
-      <c r="J79">
+        <v>334</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K79">
         <v>4</v>
       </c>
-      <c r="K79">
+      <c r="L79">
         <v>16.7</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>325</v>
       </c>
       <c r="B80" t="s">
@@ -30866,17 +31104,20 @@
         <v>300</v>
       </c>
       <c r="I80" t="s">
-        <v>333</v>
-      </c>
-      <c r="J80">
+        <v>334</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K80">
         <v>2</v>
       </c>
-      <c r="K80">
+      <c r="L80">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A81" s="7" t="s">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>325</v>
       </c>
       <c r="B81" t="s">
@@ -30901,17 +31142,20 @@
         <v>300</v>
       </c>
       <c r="I81" t="s">
-        <v>334</v>
-      </c>
-      <c r="J81">
+        <v>335</v>
+      </c>
+      <c r="J81" t="s">
+        <v>311</v>
+      </c>
+      <c r="K81">
         <v>6</v>
       </c>
-      <c r="K81">
+      <c r="L81">
         <v>21.1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>325</v>
       </c>
       <c r="B82" t="s">
@@ -30936,17 +31180,20 @@
         <v>299</v>
       </c>
       <c r="I82" t="s">
-        <v>334</v>
-      </c>
-      <c r="J82">
+        <v>335</v>
+      </c>
+      <c r="J82" t="s">
+        <v>311</v>
+      </c>
+      <c r="K82">
         <v>10</v>
       </c>
-      <c r="K82">
+      <c r="L82">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>325</v>
       </c>
       <c r="B83" t="s">
@@ -30971,17 +31218,20 @@
         <v>299</v>
       </c>
       <c r="I83" t="s">
-        <v>334</v>
-      </c>
-      <c r="J83">
+        <v>335</v>
+      </c>
+      <c r="J83" t="s">
+        <v>311</v>
+      </c>
+      <c r="K83">
         <v>2</v>
       </c>
-      <c r="K83">
+      <c r="L83">
         <v>21.84</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A84" s="7" t="s">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>325</v>
       </c>
       <c r="B84" t="s">
@@ -31006,17 +31256,20 @@
         <v>300</v>
       </c>
       <c r="I84" t="s">
-        <v>334</v>
-      </c>
-      <c r="J84">
+        <v>335</v>
+      </c>
+      <c r="J84" t="s">
+        <v>311</v>
+      </c>
+      <c r="K84">
         <v>9</v>
       </c>
-      <c r="K84">
+      <c r="L84">
         <v>23.15</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>325</v>
       </c>
       <c r="B85" t="s">
@@ -31041,17 +31294,20 @@
         <v>300</v>
       </c>
       <c r="I85" t="s">
-        <v>334</v>
-      </c>
-      <c r="J85">
+        <v>335</v>
+      </c>
+      <c r="J85" t="s">
+        <v>311</v>
+      </c>
+      <c r="K85">
         <v>12</v>
       </c>
-      <c r="K85">
+      <c r="L85">
         <v>15.97</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>325</v>
       </c>
       <c r="B86" t="s">
@@ -31076,17 +31332,20 @@
         <v>299</v>
       </c>
       <c r="I86" t="s">
-        <v>334</v>
-      </c>
-      <c r="J86">
+        <v>335</v>
+      </c>
+      <c r="J86" t="s">
+        <v>311</v>
+      </c>
+      <c r="K86">
         <v>3</v>
       </c>
-      <c r="K86">
+      <c r="L86">
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>325</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -31111,12 +31370,15 @@
         <v>299</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="J87" s="1">
+        <v>335</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="K87" s="1">
         <v>14</v>
       </c>
-      <c r="K87" s="1">
+      <c r="L87" s="1">
         <v>21.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create R Markdown for supp tables
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_seed-mix_LO.xlsx
+++ b/data/raw/from-Master_seed-mix_LO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1062" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AB3E0C2-F44D-4375-9BBE-AEFBEDD0FBDD}"/>
+  <xr:revisionPtr revIDLastSave="1063" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14CC05E5-8A67-4A77-BF66-1C403B802365}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="from-Master.xlsx" sheetId="1" r:id="rId1"/>
@@ -1116,7 +1116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1124,8 +1124,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28056,8 +28054,8 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28071,7 +28069,7 @@
     <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" customWidth="1"/>
     <col min="12" max="12" width="11.21875" customWidth="1"/>
   </cols>
@@ -28674,7 +28672,7 @@
       <c r="I16" t="s">
         <v>319</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" t="s">
         <v>310</v>
       </c>
       <c r="K16">
@@ -28712,7 +28710,7 @@
       <c r="I17" t="s">
         <v>319</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" t="s">
         <v>310</v>
       </c>
       <c r="K17">
@@ -28750,7 +28748,7 @@
       <c r="I18" t="s">
         <v>319</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" t="s">
         <v>310</v>
       </c>
       <c r="K18">
@@ -28788,7 +28786,7 @@
       <c r="I19" t="s">
         <v>319</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" t="s">
         <v>310</v>
       </c>
       <c r="K19">
@@ -28826,7 +28824,7 @@
       <c r="I20" t="s">
         <v>319</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" t="s">
         <v>310</v>
       </c>
       <c r="K20">
@@ -28864,7 +28862,7 @@
       <c r="I21" t="s">
         <v>319</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" t="s">
         <v>310</v>
       </c>
       <c r="K21">
@@ -28902,7 +28900,7 @@
       <c r="I22" t="s">
         <v>319</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" t="s">
         <v>310</v>
       </c>
       <c r="K22">
@@ -28940,7 +28938,7 @@
       <c r="I23" t="s">
         <v>317</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" t="s">
         <v>311</v>
       </c>
       <c r="K23">
@@ -28978,7 +28976,7 @@
       <c r="I24" t="s">
         <v>317</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" t="s">
         <v>311</v>
       </c>
       <c r="K24">
@@ -29016,7 +29014,7 @@
       <c r="I25" t="s">
         <v>317</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" t="s">
         <v>311</v>
       </c>
       <c r="K25">
@@ -29054,7 +29052,7 @@
       <c r="I26" t="s">
         <v>317</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" t="s">
         <v>311</v>
       </c>
       <c r="K26">
@@ -29092,7 +29090,7 @@
       <c r="I27" t="s">
         <v>317</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" t="s">
         <v>311</v>
       </c>
       <c r="K27">
@@ -29130,7 +29128,7 @@
       <c r="I28" t="s">
         <v>317</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" t="s">
         <v>311</v>
       </c>
       <c r="K28">
@@ -29168,7 +29166,7 @@
       <c r="I29" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="1" t="s">
         <v>311</v>
       </c>
       <c r="K29" s="1">
@@ -29206,7 +29204,7 @@
       <c r="I30" t="s">
         <v>320</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" t="s">
         <v>310</v>
       </c>
       <c r="K30">
@@ -29244,7 +29242,7 @@
       <c r="I31" t="s">
         <v>320</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J31" t="s">
         <v>310</v>
       </c>
       <c r="K31">
@@ -29282,7 +29280,7 @@
       <c r="I32" t="s">
         <v>320</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" t="s">
         <v>310</v>
       </c>
       <c r="K32">
@@ -29320,7 +29318,7 @@
       <c r="I33" t="s">
         <v>320</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" t="s">
         <v>310</v>
       </c>
       <c r="K33">
@@ -29358,7 +29356,7 @@
       <c r="I34" t="s">
         <v>320</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" t="s">
         <v>310</v>
       </c>
       <c r="K34">
@@ -29396,7 +29394,7 @@
       <c r="I35" t="s">
         <v>320</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" t="s">
         <v>310</v>
       </c>
       <c r="K35">
@@ -29434,7 +29432,7 @@
       <c r="I36" t="s">
         <v>320</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="J36" t="s">
         <v>310</v>
       </c>
       <c r="K36">
@@ -29472,7 +29470,7 @@
       <c r="I37" t="s">
         <v>319</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" t="s">
         <v>311</v>
       </c>
       <c r="K37">
@@ -29510,7 +29508,7 @@
       <c r="I38" t="s">
         <v>319</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" t="s">
         <v>311</v>
       </c>
       <c r="K38">
@@ -29548,7 +29546,7 @@
       <c r="I39" t="s">
         <v>319</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" t="s">
         <v>311</v>
       </c>
       <c r="K39">
@@ -29586,7 +29584,7 @@
       <c r="I40" t="s">
         <v>319</v>
       </c>
-      <c r="J40" s="5" t="s">
+      <c r="J40" t="s">
         <v>311</v>
       </c>
       <c r="K40">
@@ -29624,7 +29622,7 @@
       <c r="I41" t="s">
         <v>319</v>
       </c>
-      <c r="J41" s="5" t="s">
+      <c r="J41" t="s">
         <v>311</v>
       </c>
       <c r="K41">
@@ -29662,7 +29660,7 @@
       <c r="I42" t="s">
         <v>319</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J42" t="s">
         <v>311</v>
       </c>
       <c r="K42">
@@ -29700,7 +29698,7 @@
       <c r="I43" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="J43" s="1" t="s">
         <v>311</v>
       </c>
       <c r="K43" s="1">
@@ -29738,7 +29736,7 @@
       <c r="I44" t="s">
         <v>320</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" t="s">
         <v>310</v>
       </c>
       <c r="K44">
@@ -29776,7 +29774,7 @@
       <c r="I45" t="s">
         <v>320</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" t="s">
         <v>310</v>
       </c>
       <c r="K45">
@@ -29814,7 +29812,7 @@
       <c r="I46" t="s">
         <v>320</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J46" t="s">
         <v>310</v>
       </c>
       <c r="K46">
@@ -29852,7 +29850,7 @@
       <c r="I47" t="s">
         <v>320</v>
       </c>
-      <c r="J47" s="5" t="s">
+      <c r="J47" t="s">
         <v>310</v>
       </c>
       <c r="K47">
@@ -29890,7 +29888,7 @@
       <c r="I48" t="s">
         <v>320</v>
       </c>
-      <c r="J48" s="5" t="s">
+      <c r="J48" t="s">
         <v>310</v>
       </c>
       <c r="K48">
@@ -29928,7 +29926,7 @@
       <c r="I49" t="s">
         <v>320</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J49" t="s">
         <v>310</v>
       </c>
       <c r="K49">
@@ -29966,7 +29964,7 @@
       <c r="I50" t="s">
         <v>320</v>
       </c>
-      <c r="J50" s="5" t="s">
+      <c r="J50" t="s">
         <v>310</v>
       </c>
       <c r="K50">
@@ -30004,7 +30002,7 @@
       <c r="I51" t="s">
         <v>318</v>
       </c>
-      <c r="J51" s="5" t="s">
+      <c r="J51" t="s">
         <v>311</v>
       </c>
       <c r="K51">
@@ -30042,7 +30040,7 @@
       <c r="I52" t="s">
         <v>318</v>
       </c>
-      <c r="J52" s="5" t="s">
+      <c r="J52" t="s">
         <v>311</v>
       </c>
       <c r="K52">
@@ -30080,7 +30078,7 @@
       <c r="I53" t="s">
         <v>318</v>
       </c>
-      <c r="J53" s="5" t="s">
+      <c r="J53" t="s">
         <v>311</v>
       </c>
       <c r="K53">
@@ -30118,7 +30116,7 @@
       <c r="I54" t="s">
         <v>318</v>
       </c>
-      <c r="J54" s="5" t="s">
+      <c r="J54" t="s">
         <v>311</v>
       </c>
       <c r="K54">
@@ -30156,7 +30154,7 @@
       <c r="I55" t="s">
         <v>318</v>
       </c>
-      <c r="J55" s="5" t="s">
+      <c r="J55" t="s">
         <v>311</v>
       </c>
       <c r="K55">
@@ -30194,7 +30192,7 @@
       <c r="I56" t="s">
         <v>318</v>
       </c>
-      <c r="J56" s="5" t="s">
+      <c r="J56" t="s">
         <v>311</v>
       </c>
       <c r="K56">
@@ -30232,7 +30230,7 @@
       <c r="I57" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="J57" s="6" t="s">
+      <c r="J57" s="1" t="s">
         <v>311</v>
       </c>
       <c r="K57" s="1">
@@ -30878,7 +30876,7 @@
       <c r="I74" t="s">
         <v>334</v>
       </c>
-      <c r="J74" s="5" t="s">
+      <c r="J74" t="s">
         <v>310</v>
       </c>
       <c r="K74">
@@ -30916,7 +30914,7 @@
       <c r="I75" t="s">
         <v>334</v>
       </c>
-      <c r="J75" s="5" t="s">
+      <c r="J75" t="s">
         <v>310</v>
       </c>
       <c r="K75">
@@ -30954,7 +30952,7 @@
       <c r="I76" t="s">
         <v>334</v>
       </c>
-      <c r="J76" s="5" t="s">
+      <c r="J76" t="s">
         <v>310</v>
       </c>
       <c r="K76">
@@ -30992,7 +30990,7 @@
       <c r="I77" t="s">
         <v>334</v>
       </c>
-      <c r="J77" s="5" t="s">
+      <c r="J77" t="s">
         <v>310</v>
       </c>
       <c r="K77">
@@ -31030,7 +31028,7 @@
       <c r="I78" t="s">
         <v>334</v>
       </c>
-      <c r="J78" s="5" t="s">
+      <c r="J78" t="s">
         <v>310</v>
       </c>
       <c r="K78">
@@ -31068,7 +31066,7 @@
       <c r="I79" t="s">
         <v>334</v>
       </c>
-      <c r="J79" s="5" t="s">
+      <c r="J79" t="s">
         <v>310</v>
       </c>
       <c r="K79">
@@ -31106,7 +31104,7 @@
       <c r="I80" t="s">
         <v>334</v>
       </c>
-      <c r="J80" s="5" t="s">
+      <c r="J80" t="s">
         <v>310</v>
       </c>
       <c r="K80">

</xml_diff>